<commit_message>
Run analysis of the second essay and corrects ANOVA from the first experiment to include Bonferroni corrections.
</commit_message>
<xml_diff>
--- a/Crescimento vegetal.xlsx
+++ b/Crescimento vegetal.xlsx
@@ -245,7 +245,7 @@
     <t xml:space="preserve">id</t>
   </si>
   <si>
-    <t xml:space="preserve">colonyLength</t>
+    <t xml:space="preserve">area</t>
   </si>
   <si>
     <t xml:space="preserve">rootLength</t>
@@ -764,8 +764,8 @@
   </sheetPr>
   <dimension ref="A1:M466"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A453" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6741,9 +6741,9 @@
   <dimension ref="A1:E466"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>